<commit_message>
Fix input files for paper1 and add the experiment results to main
</commit_message>
<xml_diff>
--- a/Input/paper1-beam.xlsx
+++ b/Input/paper1-beam.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Coordinates" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,7 @@
     <sheet name="Sections" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Nodal Load" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="curve1" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="curve2" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t xml:space="preserve">Node ID</t>
   </si>
@@ -137,7 +138,7 @@
     <t xml:space="preserve">Moment Curvature Curve Sheet Name</t>
   </si>
   <si>
-    <t xml:space="preserve">curve1</t>
+    <t xml:space="preserve">curve2</t>
   </si>
   <si>
     <t xml:space="preserve">Load ID</t>
@@ -165,9 +166,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.00E+00"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -267,7 +269,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -276,15 +278,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -294,6 +296,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -368,7 +374,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -910,11 +916,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="43036084"/>
-        <c:axId val="32632343"/>
+        <c:axId val="70238166"/>
+        <c:axId val="23190032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43036084"/>
+        <c:axId val="70238166"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -956,12 +962,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32632343"/>
+        <c:crossAx val="23190032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="32632343"/>
+        <c:axId val="23190032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1003,7 +1009,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43036084"/>
+        <c:crossAx val="70238166"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1042,9 +1048,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>399240</xdr:colOff>
+      <xdr:colOff>398160</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>133200</xdr:rowOff>
+      <xdr:rowOff>132120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1052,8 +1058,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4789080" y="711720"/>
-        <a:ext cx="8665560" cy="5898240"/>
+        <a:off x="4794120" y="711720"/>
+        <a:ext cx="8678520" cy="5897160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1077,7 +1083,7 @@
       <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="16.57"/>
@@ -1269,11 +1275,11 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -1445,7 +1451,7 @@
       <c r="C7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E7" s="0" t="n">
@@ -1613,9 +1619,9 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="9.57"/>
@@ -1684,7 +1690,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.28"/>
@@ -1939,13 +1945,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.57"/>
@@ -1974,6 +1980,7 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1992,11 +1999,11 @@
   </sheetPr>
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>
@@ -2006,7 +2013,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="35.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -2022,20 +2029,20 @@
       <c r="E1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -2051,15 +2058,15 @@
       <c r="E2" s="0" t="n">
         <v>0.00036062</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <f aca="false">0.0000476881738528482/3</f>
-        <v>1.58960579509494E-005</v>
+      <c r="F2" s="3" t="n">
+        <f aca="false">E2/3</f>
+        <v>0.000120206666666667</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>1</v>
+        <v>8.27395753428702</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>-18</v>
+        <v>0</v>
       </c>
       <c r="I2" s="0" t="s">
         <v>36</v>
@@ -2070,6 +2077,7 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D23" s="5"/>
     </row>
@@ -2098,7 +2106,7 @@
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.43"/>
   </cols>
@@ -2200,13 +2208,13 @@
   </sheetPr>
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H43" activeCellId="0" sqref="H43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2796,4 +2804,100 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="69" zoomScaleNormal="69" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M40" activeCellId="0" sqref="M40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="n">
+        <v>0.000227056069745038</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2.25936502482851</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="n">
+        <v>0.000421284936640769</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>3.91959631338755</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="n">
+        <v>0.000549488533175174</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>5.98695242333847</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="n">
+        <v>0.000711478335188966</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>7.2712927918805</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="n">
+        <v>0.00253697879634439</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>13.2553977142965</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="n">
+        <v>0.00789460124147167</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>22.1555946013779</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="n">
+        <v>0.0249186673420083</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>23.0478410973136</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>